<commit_message>
Working on South-East London
</commit_message>
<xml_diff>
--- a/data/project-data.xlsx
+++ b/data/project-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan23\Documents\GitHub\ROS-Project-Map\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{960D098F-35FC-4B93-9DFE-8B0BF20A5722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B9621F-BC92-4685-BD72-D393727357E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DABD65A0-483C-4575-A0F6-9DE374C4591D}"/>
+    <workbookView xWindow="28680" yWindow="1155" windowWidth="20640" windowHeight="11160" xr2:uid="{DABD65A0-483C-4575-A0F6-9DE374C4591D}"/>
   </bookViews>
   <sheets>
     <sheet name="project-data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="183">
   <si>
     <t>Name</t>
   </si>
@@ -562,16 +562,45 @@
   </si>
   <si>
     <t>London Tilbury &amp; Southend Railway</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Parts of this interact with South London and Thameslink</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/03/West-Dulwich-to-Otford-Teynham-Sheppey-scaled.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/07/NKEDH-scaled.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/catalog/community-projects/united-kingdom/lewisham</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/12/Grove-Pk-to-Bromley-North-and-Hildenborough.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -594,19 +623,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -639,11 +686,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -659,11 +726,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -977,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DB3DEB-0EB8-4FD3-9EF9-F81EADE7405E}">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,9 +1065,10 @@
     <col min="1" max="1" width="49.5703125" customWidth="1"/>
     <col min="2" max="2" width="33.140625" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1000,8 +1078,14 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1012,7 +1096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1023,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1034,7 +1118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1045,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1056,7 +1140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1067,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1078,7 +1162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1089,7 +1173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1100,18 +1184,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>172</v>
       </c>
@@ -1122,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1133,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1144,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1155,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1166,7 +1253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1177,18 +1264,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1199,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1210,7 +1300,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1221,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1232,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1243,7 +1333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1254,7 +1344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1265,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1276,7 +1366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1287,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1298,7 +1388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1309,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -1320,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -1331,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1342,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -1353,7 +1443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -1364,7 +1454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -1375,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -1386,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -1397,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -1408,7 +1498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -1419,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -1430,7 +1520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -1440,8 +1530,11 @@
       <c r="C41" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -1452,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -1463,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -1474,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -1485,7 +1578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -1496,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -1507,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -1518,7 +1611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>95</v>
       </c>
@@ -1529,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>97</v>
       </c>
@@ -1540,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>99</v>
       </c>
@@ -1551,7 +1644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>101</v>
       </c>
@@ -1562,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>103</v>
       </c>
@@ -1573,7 +1666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>105</v>
       </c>
@@ -1584,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>107</v>
       </c>
@@ -1595,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>175</v>
       </c>
@@ -1606,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>110</v>
       </c>
@@ -1617,7 +1710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -1628,7 +1721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -1636,10 +1729,13 @@
         <v>114</v>
       </c>
       <c r="C59" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>115</v>
       </c>
@@ -1650,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -1661,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>174</v>
       </c>
@@ -1672,7 +1768,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>120</v>
       </c>
@@ -1683,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>122</v>
       </c>
@@ -1694,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>124</v>
       </c>
@@ -1705,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>126</v>
       </c>
@@ -1716,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>128</v>
       </c>
@@ -1727,18 +1823,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>130</v>
       </c>
       <c r="B68" t="s">
         <v>131</v>
       </c>
-      <c r="C68" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>132</v>
       </c>
@@ -1749,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>134</v>
       </c>
@@ -1760,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>136</v>
       </c>
@@ -1771,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>138</v>
       </c>
@@ -1782,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>140</v>
       </c>
@@ -1793,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>142</v>
       </c>
@@ -1804,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>144</v>
       </c>
@@ -1815,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>146</v>
       </c>
@@ -1826,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>148</v>
       </c>
@@ -1837,7 +1936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>150</v>
       </c>
@@ -1848,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>152</v>
       </c>
@@ -1859,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>154</v>
       </c>
@@ -1960,6 +2059,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C1048576">
+    <cfRule type="iconSet" priority="7">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"WIP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="iconSet" priority="5">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="num" val="TRUE"/>
+      </iconSet>
+    </cfRule>
     <cfRule type="iconSet" priority="6">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -1968,32 +2092,17 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"WIP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="iconSet" priority="4">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="num" val="TRUE"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="5">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{27C35F13-2332-4ADD-AE84-E0315758E4E1}"/>
+    <hyperlink ref="D41" r:id="rId2" xr:uid="{4DCA43D3-DFC4-4C5D-A2F4-D33BA5444378}"/>
+    <hyperlink ref="D59" r:id="rId3" xr:uid="{1177B9A5-E58D-41B0-B8B0-8BC9E84B3ECD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on SE London
</commit_message>
<xml_diff>
--- a/data/project-data.xlsx
+++ b/data/project-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan23\Documents\GitHub\ROS-Project-Map\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B9621F-BC92-4685-BD72-D393727357E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791C266B-D041-4806-992E-49501EB7C3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1155" windowWidth="20640" windowHeight="11160" xr2:uid="{DABD65A0-483C-4575-A0F6-9DE374C4591D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DABD65A0-483C-4575-A0F6-9DE374C4591D}"/>
   </bookViews>
   <sheets>
     <sheet name="project-data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="190">
   <si>
     <t>Name</t>
   </si>
@@ -583,6 +583,27 @@
   </si>
   <si>
     <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/12/Grove-Pk-to-Bromley-North-and-Hildenborough.png</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/02/Swanley-scaled.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/07/Charing-Cross-Canon-St-London-Bridge-scaled.jpg</t>
+  </si>
+  <si>
+    <t>Not including this project</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/02/Victoria-Central-Workstation-2.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/02/Victoria-Central-Workstation-1.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2019/06/Victoria-South-Eastern-scaled.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2021/10/SouthLondonAndThameslink-scaled.bmp</t>
   </si>
 </sst>
 </file>
@@ -643,7 +664,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -651,66 +672,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1056,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DB3DEB-0EB8-4FD3-9EF9-F81EADE7405E}">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,6 +1213,9 @@
       <c r="C16" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D16" s="3" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1263,6 +1227,9 @@
       <c r="C17" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D17" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1274,6 +1241,9 @@
       <c r="C18" s="1" t="s">
         <v>173</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>186</v>
+      </c>
       <c r="E18" t="s">
         <v>177</v>
       </c>
@@ -1310,6 +1280,12 @@
       <c r="C21" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="D21" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E21" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1398,6 +1374,9 @@
       <c r="C29" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="D29" s="3" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1527,8 +1506,8 @@
       <c r="B41" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>173</v>
+      <c r="C41" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>180</v>
@@ -1833,7 +1812,7 @@
       <c r="C68" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="2" t="s">
         <v>182</v>
       </c>
     </row>
@@ -1969,7 +1948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>156</v>
       </c>
@@ -1980,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>158</v>
       </c>
@@ -1991,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>160</v>
       </c>
@@ -2002,7 +1981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>162</v>
       </c>
@@ -2013,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>164</v>
       </c>
@@ -2024,18 +2003,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>166</v>
       </c>
       <c r="B86" t="s">
         <v>167</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>168</v>
       </c>
@@ -2046,7 +2028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>170</v>
       </c>
@@ -2068,13 +2050,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="iconSet" priority="5">
@@ -2101,8 +2083,9 @@
     <hyperlink ref="D11" r:id="rId1" xr:uid="{27C35F13-2332-4ADD-AE84-E0315758E4E1}"/>
     <hyperlink ref="D41" r:id="rId2" xr:uid="{4DCA43D3-DFC4-4C5D-A2F4-D33BA5444378}"/>
     <hyperlink ref="D59" r:id="rId3" xr:uid="{1177B9A5-E58D-41B0-B8B0-8BC9E84B3ECD}"/>
+    <hyperlink ref="D68" r:id="rId4" xr:uid="{62E679E0-880C-4BF3-92A0-C18FFB52BB3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Expanding South of London
</commit_message>
<xml_diff>
--- a/data/project-data.xlsx
+++ b/data/project-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan23\Documents\GitHub\ROS-Project-Map\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791C266B-D041-4806-992E-49501EB7C3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB410D1E-DF0A-4E96-B533-37F58607BF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DABD65A0-483C-4575-A0F6-9DE374C4591D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="200">
   <si>
     <t>Name</t>
   </si>
@@ -150,12 +150,6 @@
     <t>Victoria Central (Workstation 2)</t>
   </si>
   <si>
-    <t>Toronto Subway</t>
-  </si>
-  <si>
-    <t>Canada, Community Project, Community Projects, Matt Burb, Metro, North America, Toronto, Underground</t>
-  </si>
-  <si>
     <t>Thameslink Core</t>
   </si>
   <si>
@@ -249,12 +243,6 @@
     <t>Blackpool, Community Project, Community Projects, Craig Weekes, Preston, United Kingdom</t>
   </si>
   <si>
-    <t>Port Authority Trans-Hudson (PATH)</t>
-  </si>
-  <si>
-    <t>Community Project, Community Projects, Krizar, New York, North America, PATH</t>
-  </si>
-  <si>
     <t>District Line – Western Area</t>
   </si>
   <si>
@@ -582,9 +570,6 @@
     <t>https://www.railwayoperationsimulator.com/catalog/community-projects/united-kingdom/lewisham</t>
   </si>
   <si>
-    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/12/Grove-Pk-to-Bromley-North-and-Hildenborough.png</t>
-  </si>
-  <si>
     <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/02/Swanley-scaled.jpg</t>
   </si>
   <si>
@@ -604,6 +589,51 @@
   </si>
   <si>
     <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2021/10/SouthLondonAndThameslink-scaled.bmp</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2021/02/ClaphamJunction.bmp</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2021/08/Waterloo-980x318.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2020/11/WaterlooSuburban-1-980x386.png</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2020/06/Fareham.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2017/10/Guildford.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2021/05/Portsmouth-Direct-Line.bmp</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2020/03/Newport-screenshot.png</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/06/Southampton-Central.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2020/02/BarnhamandFord.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/catalog/community-projects/united-kingdom/grove-park-hildenborough-and-ashford</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>This project is in 3 sections - map in separate colours</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/02/WokingASCv32-scaled.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2012/02/Basingstoke-scaled.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2013/02/Railway-Image-Reading-2020-scaled.jpg</t>
   </si>
 </sst>
 </file>
@@ -664,7 +694,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -705,6 +735,12 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -716,6 +752,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FC6B679D-1FCA-49BE-8A36-F59620C99EB8}" name="Table1" displayName="Table1" ref="A1:E86" totalsRowShown="0">
+  <autoFilter ref="A1:E86" xr:uid="{FC6B679D-1FCA-49BE-8A36-F59620C99EB8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E86">
+    <sortCondition ref="A1:A86"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{F1E29613-AEDA-4F80-A07C-0034D358E89C}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{B97CB56D-101F-4958-B986-C01C014305A1}" name="Tags"/>
+    <tableColumn id="3" xr3:uid="{8EB0951B-536C-46AF-A6D3-CAE4AA26E548}" name="Added to map?" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{EEB18F33-2716-411A-B364-7A12EF0925D3}" name="Link" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{D5EF4736-10A8-4D6A-B209-5897B4049F98}" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1015,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DB3DEB-0EB8-4FD3-9EF9-F81EADE7405E}">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1079,8 @@
     <col min="1" max="1" width="49.5703125" customWidth="1"/>
     <col min="2" max="2" width="33.140625" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19" style="3" customWidth="1"/>
+    <col min="5" max="5" width="59" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1040,10 +1094,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1070,10 +1124,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>0</v>
@@ -1081,10 +1135,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>0</v>
@@ -1092,32 +1146,44 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E7" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>0</v>
@@ -1147,24 +1213,21 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>179</v>
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>0</v>
@@ -1172,10 +1235,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="b">
         <v>0</v>
@@ -1183,10 +1246,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="b">
         <v>0</v>
@@ -1194,10 +1257,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>166</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>167</v>
       </c>
       <c r="C15" s="1" t="b">
         <v>0</v>
@@ -1205,94 +1268,88 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>188</v>
+        <v>179</v>
+      </c>
+      <c r="E16" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1" t="b">
         <v>0</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>144</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="E18" t="s">
-        <v>177</v>
+        <v>145</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="C19" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E19" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>173</v>
+        <v>60</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>140</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>141</v>
       </c>
       <c r="C21" s="1" t="b">
         <v>0</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="E21" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>0</v>
@@ -1300,10 +1357,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="C23" s="1" t="b">
         <v>0</v>
@@ -1311,10 +1368,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="C24" s="1" t="b">
         <v>0</v>
@@ -1322,10 +1379,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C25" s="1" t="b">
         <v>0</v>
@@ -1333,10 +1390,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="C26" s="1" t="b">
         <v>0</v>
@@ -1344,10 +1401,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="C27" s="1" t="b">
         <v>0</v>
@@ -1355,10 +1412,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="C28" s="1" t="b">
         <v>0</v>
@@ -1366,24 +1423,21 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>137</v>
       </c>
       <c r="C29" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>184</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>164</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="C30" s="1" t="b">
         <v>0</v>
@@ -1391,651 +1445,725 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="C31" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E31" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="C32" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>129</v>
       </c>
       <c r="C33" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="C34" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>131</v>
       </c>
       <c r="C35" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E36" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="C37" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E37" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="C38" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>170</v>
+      </c>
+      <c r="B40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>158</v>
+      </c>
+      <c r="B41" t="s">
+        <v>159</v>
+      </c>
+      <c r="C41" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>150</v>
+      </c>
+      <c r="B44" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E45" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>171</v>
+      </c>
+      <c r="B48" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>156</v>
+      </c>
+      <c r="B50" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E50" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" t="s">
+        <v>83</v>
+      </c>
+      <c r="C56" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E58" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s">
         <v>77</v>
-      </c>
-      <c r="B39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>79</v>
-      </c>
-      <c r="B40" t="s">
-        <v>80</v>
-      </c>
-      <c r="C40" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" t="s">
-        <v>92</v>
-      </c>
-      <c r="C47" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>93</v>
-      </c>
-      <c r="B48" t="s">
-        <v>94</v>
-      </c>
-      <c r="C48" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>95</v>
-      </c>
-      <c r="B49" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" t="s">
-        <v>98</v>
-      </c>
-      <c r="C50" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>99</v>
-      </c>
-      <c r="B51" t="s">
-        <v>100</v>
-      </c>
-      <c r="C51" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>101</v>
-      </c>
-      <c r="B52" t="s">
-        <v>102</v>
-      </c>
-      <c r="C52" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>103</v>
-      </c>
-      <c r="B53" t="s">
-        <v>104</v>
-      </c>
-      <c r="C53" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>105</v>
-      </c>
-      <c r="B54" t="s">
-        <v>106</v>
-      </c>
-      <c r="C54" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>107</v>
-      </c>
-      <c r="B55" t="s">
-        <v>108</v>
-      </c>
-      <c r="C55" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>175</v>
-      </c>
-      <c r="B56" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>110</v>
-      </c>
-      <c r="B57" t="s">
-        <v>111</v>
-      </c>
-      <c r="C57" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>112</v>
-      </c>
-      <c r="B58" t="s">
-        <v>113</v>
-      </c>
-      <c r="C58" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>2</v>
-      </c>
-      <c r="B59" t="s">
-        <v>114</v>
       </c>
       <c r="C59" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E59" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60" t="s">
+        <v>76</v>
+      </c>
+      <c r="C60" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>152</v>
+      </c>
+      <c r="B62" t="s">
+        <v>153</v>
+      </c>
+      <c r="C62" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>154</v>
+      </c>
+      <c r="B63" t="s">
+        <v>155</v>
+      </c>
+      <c r="C63" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>146</v>
+      </c>
+      <c r="B64" t="s">
+        <v>147</v>
+      </c>
+      <c r="C64" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E64" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>66</v>
+      </c>
+      <c r="C66" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>61</v>
+      </c>
+      <c r="B68" t="s">
+        <v>62</v>
+      </c>
+      <c r="C68" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E68" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>148</v>
+      </c>
+      <c r="B69" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>48</v>
+      </c>
+      <c r="B70" t="s">
+        <v>47</v>
+      </c>
+      <c r="C70" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>46</v>
+      </c>
+      <c r="B71" t="s">
+        <v>47</v>
+      </c>
+      <c r="C71" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>44</v>
+      </c>
+      <c r="B72" t="s">
+        <v>45</v>
+      </c>
+      <c r="C72" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>162</v>
+      </c>
+      <c r="B73" t="s">
+        <v>163</v>
+      </c>
+      <c r="C73" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E73" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>42</v>
+      </c>
+      <c r="B74" t="s">
+        <v>43</v>
+      </c>
+      <c r="C74" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E74" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>40</v>
+      </c>
+      <c r="B75" t="s">
+        <v>41</v>
+      </c>
+      <c r="C75" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E75" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>38</v>
+      </c>
+      <c r="B76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>35</v>
+      </c>
+      <c r="B77" t="s">
+        <v>36</v>
+      </c>
+      <c r="C77" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E77" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>37</v>
+      </c>
+      <c r="B78" t="s">
+        <v>36</v>
+      </c>
+      <c r="C78" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>115</v>
-      </c>
-      <c r="B60" t="s">
-        <v>116</v>
-      </c>
-      <c r="C60" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>117</v>
-      </c>
-      <c r="B61" t="s">
-        <v>118</v>
-      </c>
-      <c r="C61" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>174</v>
-      </c>
-      <c r="B62" t="s">
-        <v>119</v>
-      </c>
-      <c r="C62" s="1" t="s">
+      <c r="E78" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>120</v>
-      </c>
-      <c r="B63" t="s">
-        <v>121</v>
-      </c>
-      <c r="C63" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>122</v>
-      </c>
-      <c r="B64" t="s">
-        <v>123</v>
-      </c>
-      <c r="C64" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>124</v>
-      </c>
-      <c r="B65" t="s">
-        <v>125</v>
-      </c>
-      <c r="C65" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>126</v>
-      </c>
-      <c r="B66" t="s">
-        <v>127</v>
-      </c>
-      <c r="C66" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>128</v>
-      </c>
-      <c r="B67" t="s">
-        <v>129</v>
-      </c>
-      <c r="C67" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>130</v>
-      </c>
-      <c r="B68" t="s">
-        <v>131</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>132</v>
-      </c>
-      <c r="B69" t="s">
-        <v>133</v>
-      </c>
-      <c r="C69" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>33</v>
+      </c>
+      <c r="B79" t="s">
+        <v>34</v>
+      </c>
+      <c r="C79" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E79" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>138</v>
+      </c>
+      <c r="B80" t="s">
+        <v>139</v>
+      </c>
+      <c r="C80" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>168</v>
+      </c>
+      <c r="B81" t="s">
+        <v>26</v>
+      </c>
+      <c r="C81" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>134</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B82" t="s">
         <v>135</v>
       </c>
-      <c r="C70" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>136</v>
-      </c>
-      <c r="B71" t="s">
-        <v>137</v>
-      </c>
-      <c r="C71" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>138</v>
-      </c>
-      <c r="B72" t="s">
-        <v>139</v>
-      </c>
-      <c r="C72" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>140</v>
-      </c>
-      <c r="B73" t="s">
-        <v>141</v>
-      </c>
-      <c r="C73" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>142</v>
-      </c>
-      <c r="B74" t="s">
-        <v>143</v>
-      </c>
-      <c r="C74" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>144</v>
-      </c>
-      <c r="B75" t="s">
-        <v>145</v>
-      </c>
-      <c r="C75" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>146</v>
-      </c>
-      <c r="B76" t="s">
-        <v>147</v>
-      </c>
-      <c r="C76" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>148</v>
-      </c>
-      <c r="B77" t="s">
-        <v>149</v>
-      </c>
-      <c r="C77" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>150</v>
-      </c>
-      <c r="B78" t="s">
-        <v>151</v>
-      </c>
-      <c r="C78" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>152</v>
-      </c>
-      <c r="B79" t="s">
-        <v>153</v>
-      </c>
-      <c r="C79" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>154</v>
-      </c>
-      <c r="B80" t="s">
-        <v>155</v>
-      </c>
-      <c r="C80" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>156</v>
-      </c>
-      <c r="B81" t="s">
-        <v>157</v>
-      </c>
-      <c r="C81" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>158</v>
-      </c>
-      <c r="B82" t="s">
-        <v>159</v>
-      </c>
       <c r="C82" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E82" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>160</v>
+        <v>24</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
-      </c>
-      <c r="C83" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E83" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>162</v>
+        <v>31</v>
       </c>
       <c r="B84" t="s">
-        <v>163</v>
+        <v>32</v>
       </c>
       <c r="C84" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E84" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
       <c r="B85" t="s">
-        <v>165</v>
+        <v>30</v>
       </c>
       <c r="C85" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>166</v>
+        <v>18</v>
       </c>
       <c r="B86" t="s">
-        <v>167</v>
+        <v>19</v>
       </c>
       <c r="C86" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>168</v>
-      </c>
-      <c r="B87" t="s">
-        <v>169</v>
-      </c>
-      <c r="C87" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>170</v>
-      </c>
-      <c r="B88" t="s">
-        <v>171</v>
-      </c>
-      <c r="C88" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2080,12 +2208,14 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" xr:uid="{27C35F13-2332-4ADD-AE84-E0315758E4E1}"/>
-    <hyperlink ref="D41" r:id="rId2" xr:uid="{4DCA43D3-DFC4-4C5D-A2F4-D33BA5444378}"/>
-    <hyperlink ref="D59" r:id="rId3" xr:uid="{1177B9A5-E58D-41B0-B8B0-8BC9E84B3ECD}"/>
-    <hyperlink ref="D68" r:id="rId4" xr:uid="{62E679E0-880C-4BF3-92A0-C18FFB52BB3C}"/>
+    <hyperlink ref="D83" r:id="rId1" xr:uid="{27C35F13-2332-4ADD-AE84-E0315758E4E1}"/>
+    <hyperlink ref="D59" r:id="rId2" xr:uid="{4DCA43D3-DFC4-4C5D-A2F4-D33BA5444378}"/>
+    <hyperlink ref="D45" r:id="rId3" xr:uid="{1177B9A5-E58D-41B0-B8B0-8BC9E84B3ECD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished Kent and the South-East
</commit_message>
<xml_diff>
--- a/data/project-data.xlsx
+++ b/data/project-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan23\Documents\GitHub\ROS-Project-Map\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB410D1E-DF0A-4E96-B533-37F58607BF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747BE13F-1074-450E-8B77-30A2F69BD85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DABD65A0-483C-4575-A0F6-9DE374C4591D}"/>
+    <workbookView xWindow="-21720" yWindow="2430" windowWidth="21840" windowHeight="13140" xr2:uid="{DABD65A0-483C-4575-A0F6-9DE374C4591D}"/>
   </bookViews>
   <sheets>
     <sheet name="project-data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="202">
   <si>
     <t>Name</t>
   </si>
@@ -634,6 +634,12 @@
   </si>
   <si>
     <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2013/02/Railway-Image-Reading-2020-scaled.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/04/Eastbourne-Seaford-and-Newhaven-scaled.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2020/04/Faversham-to-Ramsgate.jpg</t>
   </si>
 </sst>
 </file>
@@ -696,6 +702,12 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -735,12 +747,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -763,8 +769,8 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{F1E29613-AEDA-4F80-A07C-0034D358E89C}" name="Name"/>
     <tableColumn id="2" xr3:uid="{B97CB56D-101F-4958-B986-C01C014305A1}" name="Tags"/>
-    <tableColumn id="3" xr3:uid="{8EB0951B-536C-46AF-A6D3-CAE4AA26E548}" name="Added to map?" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{EEB18F33-2716-411A-B364-7A12EF0925D3}" name="Link" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{8EB0951B-536C-46AF-A6D3-CAE4AA26E548}" name="Added to map?" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{EEB18F33-2716-411A-B364-7A12EF0925D3}" name="Link" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{D5EF4736-10A8-4D6A-B209-5897B4049F98}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1070,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DB3DEB-0EB8-4FD3-9EF9-F81EADE7405E}">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,7 +1424,13 @@
         <v>4</v>
       </c>
       <c r="C28" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E28" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1468,7 +1480,13 @@
         <v>125</v>
       </c>
       <c r="C32" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E32" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1481,6 +1499,9 @@
       <c r="C33" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="E33" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1511,8 +1532,8 @@
       <c r="B36" t="s">
         <v>127</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>169</v>
+      <c r="C36" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>194</v>
@@ -2178,13 +2199,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="iconSet" priority="5">
@@ -2203,7 +2224,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2211,11 +2232,13 @@
     <hyperlink ref="D83" r:id="rId1" xr:uid="{27C35F13-2332-4ADD-AE84-E0315758E4E1}"/>
     <hyperlink ref="D59" r:id="rId2" xr:uid="{4DCA43D3-DFC4-4C5D-A2F4-D33BA5444378}"/>
     <hyperlink ref="D45" r:id="rId3" xr:uid="{1177B9A5-E58D-41B0-B8B0-8BC9E84B3ECD}"/>
+    <hyperlink ref="D36" r:id="rId4" xr:uid="{F42D7F6F-9FE8-4E54-8FBE-DDEEAD186D0C}"/>
+    <hyperlink ref="D28" r:id="rId5" xr:uid="{7AF0D795-BA2A-49D8-8AE2-82CDA105C9B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a little to the map
</commit_message>
<xml_diff>
--- a/data/project-data.xlsx
+++ b/data/project-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan23\Documents\GitHub\ROS-Project-Map\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747BE13F-1074-450E-8B77-30A2F69BD85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BB4AE7-7098-4EC0-92CF-1505B48F2882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2430" windowWidth="21840" windowHeight="13140" xr2:uid="{DABD65A0-483C-4575-A0F6-9DE374C4591D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="200">
   <si>
     <t>Name</t>
   </si>
@@ -508,12 +508,6 @@
   </si>
   <si>
     <t>Community Project, Community Projects, Daniel Gill, London Waterloo, UK</t>
-  </si>
-  <si>
-    <t>HS2 Demonstration London</t>
-  </si>
-  <si>
-    <t>Community Project, Community Projects, Daniel Gill, London, United Kingdom</t>
   </si>
   <si>
     <t>Antwerpen-Centraal</t>
@@ -761,10 +755,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FC6B679D-1FCA-49BE-8A36-F59620C99EB8}" name="Table1" displayName="Table1" ref="A1:E86" totalsRowShown="0">
-  <autoFilter ref="A1:E86" xr:uid="{FC6B679D-1FCA-49BE-8A36-F59620C99EB8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E86">
-    <sortCondition ref="A1:A86"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FC6B679D-1FCA-49BE-8A36-F59620C99EB8}" name="Table1" displayName="Table1" ref="A1:E85" totalsRowShown="0">
+  <autoFilter ref="A1:E85" xr:uid="{FC6B679D-1FCA-49BE-8A36-F59620C99EB8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E85">
+    <sortCondition ref="A1:A85"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{F1E29613-AEDA-4F80-A07C-0034D358E89C}" name="Name"/>
@@ -1074,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DB3DEB-0EB8-4FD3-9EF9-F81EADE7405E}">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,10 +1094,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1130,10 +1124,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>0</v>
@@ -1158,13 +1152,13 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6" t="s">
         <v>193</v>
-      </c>
-      <c r="E6" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1178,10 +1172,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1263,10 +1257,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C15" s="1" t="b">
         <v>0</v>
@@ -1283,10 +1277,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1322,10 +1316,10 @@
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1427,10 +1421,10 @@
         <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1446,10 +1440,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C30" s="1" t="b">
         <v>0</v>
@@ -1466,10 +1460,10 @@
         <v>0</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,10 +1477,10 @@
         <v>1</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1500,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1536,10 +1530,10 @@
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E36" t="s">
         <v>194</v>
-      </c>
-      <c r="E36" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1550,13 +1544,13 @@
         <v>121</v>
       </c>
       <c r="C37" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E37" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1583,21 +1577,21 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B40" t="s">
         <v>115</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>158</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
       <c r="C41" s="1" t="b">
         <v>0</v>
@@ -1605,10 +1599,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B42" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C42" s="1" t="b">
         <v>0</v>
@@ -1616,10 +1610,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="C43" s="1" t="b">
         <v>0</v>
@@ -1627,38 +1621,38 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>150</v>
+        <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="C44" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E44" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>2</v>
+        <v>108</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C45" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E45" t="s">
-        <v>195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B46" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C46" s="1" t="b">
         <v>0</v>
@@ -1666,10 +1660,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>169</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C47" s="1" t="b">
         <v>0</v>
@@ -1677,10 +1671,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>171</v>
+        <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C48" s="1" t="b">
         <v>0</v>
@@ -1688,38 +1682,38 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>103</v>
+        <v>156</v>
       </c>
       <c r="B49" t="s">
-        <v>104</v>
+        <v>157</v>
       </c>
       <c r="C49" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E49" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>156</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>157</v>
+        <v>102</v>
       </c>
       <c r="C50" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="E50" t="s">
-        <v>195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C51" s="1" t="b">
         <v>0</v>
@@ -1727,10 +1721,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C52" s="1" t="b">
         <v>0</v>
@@ -1738,10 +1732,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B53" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C53" s="1" t="b">
         <v>0</v>
@@ -1749,10 +1743,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C54" s="1" t="b">
         <v>0</v>
@@ -1760,10 +1754,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B55" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C55" s="1" t="b">
         <v>0</v>
@@ -1771,10 +1765,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C56" s="1" t="b">
         <v>0</v>
@@ -1782,55 +1776,55 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B57" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C57" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E57" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C58" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>191</v>
+        <v>1</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="E58" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E59" t="s">
-        <v>195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B60" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C60" s="1" t="b">
         <v>0</v>
@@ -1838,10 +1832,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>152</v>
       </c>
       <c r="B61" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="C61" s="1" t="b">
         <v>0</v>
@@ -1849,10 +1843,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B62" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C62" s="1" t="b">
         <v>0</v>
@@ -1860,38 +1854,38 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B63" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C63" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E63" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>146</v>
+        <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>147</v>
+        <v>68</v>
       </c>
       <c r="C64" s="1" t="b">
         <v>0</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E64" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C65" s="1" t="b">
         <v>0</v>
@@ -1899,10 +1893,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C66" s="1" t="b">
         <v>0</v>
@@ -1910,38 +1904,38 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C67" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E67" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>61</v>
+        <v>148</v>
       </c>
       <c r="B68" t="s">
-        <v>62</v>
+        <v>149</v>
       </c>
       <c r="C68" s="1" t="b">
         <v>0</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E68" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>148</v>
+        <v>48</v>
       </c>
       <c r="B69" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
       <c r="C69" s="1" t="b">
         <v>0</v>
@@ -1949,7 +1943,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B70" t="s">
         <v>47</v>
@@ -1960,10 +1954,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B71" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C71" s="1" t="b">
         <v>0</v>
@@ -1971,80 +1965,86 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>44</v>
+        <v>160</v>
       </c>
       <c r="B72" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="C72" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E72" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
       <c r="B73" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="C73" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="E73" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C74" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="E74" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B75" t="s">
-        <v>41</v>
-      </c>
-      <c r="C75" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E75" t="s">
-        <v>180</v>
+        <v>39</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B76" t="s">
-        <v>39</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>169</v>
+        <v>36</v>
+      </c>
+      <c r="C76" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E76" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B77" t="s">
         <v>36</v>
@@ -2053,18 +2053,18 @@
         <v>1</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E77" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B78" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C78" s="1" t="b">
         <v>1</v>
@@ -2073,32 +2073,26 @@
         <v>181</v>
       </c>
       <c r="E78" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="B79" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="C79" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="E79" t="s">
-        <v>195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="B80" t="s">
-        <v>139</v>
+        <v>26</v>
       </c>
       <c r="C80" s="1" t="b">
         <v>0</v>
@@ -2106,85 +2100,74 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="B81" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="C81" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E81" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>134</v>
+        <v>24</v>
       </c>
       <c r="B82" t="s">
-        <v>135</v>
+        <v>25</v>
       </c>
       <c r="C82" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>187</v>
+        <v>1</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="E82" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B83" t="s">
-        <v>25</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>175</v>
+        <v>32</v>
+      </c>
+      <c r="C83" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="E83" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B84" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C84" s="1" t="b">
         <v>0</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="E84" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B85" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C85" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>18</v>
-      </c>
-      <c r="B86" t="s">
-        <v>19</v>
-      </c>
-      <c r="C86" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2229,9 +2212,9 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D83" r:id="rId1" xr:uid="{27C35F13-2332-4ADD-AE84-E0315758E4E1}"/>
-    <hyperlink ref="D59" r:id="rId2" xr:uid="{4DCA43D3-DFC4-4C5D-A2F4-D33BA5444378}"/>
-    <hyperlink ref="D45" r:id="rId3" xr:uid="{1177B9A5-E58D-41B0-B8B0-8BC9E84B3ECD}"/>
+    <hyperlink ref="D82" r:id="rId1" xr:uid="{27C35F13-2332-4ADD-AE84-E0315758E4E1}"/>
+    <hyperlink ref="D58" r:id="rId2" xr:uid="{4DCA43D3-DFC4-4C5D-A2F4-D33BA5444378}"/>
+    <hyperlink ref="D44" r:id="rId3" xr:uid="{1177B9A5-E58D-41B0-B8B0-8BC9E84B3ECD}"/>
     <hyperlink ref="D36" r:id="rId4" xr:uid="{F42D7F6F-9FE8-4E54-8FBE-DDEEAD186D0C}"/>
     <hyperlink ref="D28" r:id="rId5" xr:uid="{7AF0D795-BA2A-49D8-8AE2-82CDA105C9B0}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Almost done with South Wales
</commit_message>
<xml_diff>
--- a/data/project-data.xlsx
+++ b/data/project-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan23\Documents\GitHub\ROS-Project-Map\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEB8187-8BBC-4D5F-A7FE-184E1A7ECD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E86F9B-9452-46A0-9D25-908DE8354FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1155" windowWidth="20640" windowHeight="11160" xr2:uid="{DABD65A0-483C-4575-A0F6-9DE374C4591D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="234">
   <si>
     <t>Name</t>
   </si>
@@ -1162,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DB3DEB-0EB8-4FD3-9EF9-F81EADE7405E}">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,7 +1347,7 @@
         <v>48</v>
       </c>
       <c r="C11" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>232</v>
@@ -2054,8 +2054,8 @@
       <c r="B59" t="s">
         <v>86</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>159</v>
+      <c r="C59" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>181</v>

</xml_diff>

<commit_message>
Moving into the Heart of England
</commit_message>
<xml_diff>
--- a/data/project-data.xlsx
+++ b/data/project-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan23\Documents\GitHub\ROS-Project-Map\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E86F9B-9452-46A0-9D25-908DE8354FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E45D12F-030B-44E1-A282-DD63E1E3DD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1155" windowWidth="20640" windowHeight="11160" xr2:uid="{DABD65A0-483C-4575-A0F6-9DE374C4591D}"/>
+    <workbookView xWindow="-21720" yWindow="2430" windowWidth="21840" windowHeight="13140" xr2:uid="{DABD65A0-483C-4575-A0F6-9DE374C4591D}"/>
   </bookViews>
   <sheets>
     <sheet name="project-data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="235">
   <si>
     <t>Name</t>
   </si>
@@ -736,6 +736,9 @@
   </si>
   <si>
     <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/02/Cambrian-scaled.jpg</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2020/10/Cornwall-update.jpg</t>
   </si>
 </sst>
 </file>
@@ -1162,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DB3DEB-0EB8-4FD3-9EF9-F81EADE7405E}">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,7 +1477,13 @@
         <v>56</v>
       </c>
       <c r="C19" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E19" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added missing latest projects
</commit_message>
<xml_diff>
--- a/data/project-data.xlsx
+++ b/data/project-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan23\Documents\GitHub\ROS-Project-Map\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E45D12F-030B-44E1-A282-DD63E1E3DD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C33421A-0155-49CE-859A-3268237EA9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="2430" windowWidth="21840" windowHeight="13140" xr2:uid="{DABD65A0-483C-4575-A0F6-9DE374C4591D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DABD65A0-483C-4575-A0F6-9DE374C4591D}"/>
   </bookViews>
   <sheets>
     <sheet name="project-data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="237">
   <si>
     <t>Name</t>
   </si>
@@ -144,12 +144,6 @@
     <t>Community Project, Community Projects, London, Oxalin, Thameslink, United Kingdom</t>
   </si>
   <si>
-    <t>Swanley</t>
-  </si>
-  <si>
-    <t>Community Project, Community Projects, Craig Weekes, Swanley, United Kingdom</t>
-  </si>
-  <si>
     <t>Southampton Central</t>
   </si>
   <si>
@@ -540,9 +534,6 @@
     <t>https://www.railwayoperationsimulator.com/catalog/community-projects/united-kingdom/lewisham</t>
   </si>
   <si>
-    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/02/Swanley-scaled.jpg</t>
-  </si>
-  <si>
     <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2018/07/Charing-Cross-Canon-St-London-Bridge-scaled.jpg</t>
   </si>
   <si>
@@ -739,6 +730,21 @@
   </si>
   <si>
     <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2020/10/Cornwall-update.jpg</t>
+  </si>
+  <si>
+    <t>Chatham/Southeastern Main Line Chislehurst Junction – Shortlands to Swanley &amp; Grove Park to Petts Wood</t>
+  </si>
+  <si>
+    <t>MissCatTrap</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2022/02/ChathamMainLine-Chislehurst-Light.jpg</t>
+  </si>
+  <si>
+    <t>Chatham Main Line Rochester to Faversham + Medway Valley &amp; Sheerness</t>
+  </si>
+  <si>
+    <t>https://www.railwayoperationsimulator.com/wp-content/uploads/2022/02/ChathamMainLine-Medway.bmp</t>
   </si>
 </sst>
 </file>
@@ -801,12 +807,6 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -836,6 +836,12 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -850,16 +856,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FC6B679D-1FCA-49BE-8A36-F59620C99EB8}" name="Table1" displayName="Table1" ref="A1:E156" totalsRowShown="0">
-  <autoFilter ref="A1:E156" xr:uid="{FC6B679D-1FCA-49BE-8A36-F59620C99EB8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E90">
-    <sortCondition ref="A1:A156"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FC6B679D-1FCA-49BE-8A36-F59620C99EB8}" name="Table1" displayName="Table1" ref="A1:E155" totalsRowShown="0">
+  <autoFilter ref="A1:E155" xr:uid="{FC6B679D-1FCA-49BE-8A36-F59620C99EB8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E89">
+    <sortCondition ref="A1:A155"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{F1E29613-AEDA-4F80-A07C-0034D358E89C}" name="Name"/>
     <tableColumn id="2" xr3:uid="{B97CB56D-101F-4958-B986-C01C014305A1}" name="Tags"/>
-    <tableColumn id="3" xr3:uid="{8EB0951B-536C-46AF-A6D3-CAE4AA26E548}" name="Added to map?" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{EEB18F33-2716-411A-B364-7A12EF0925D3}" name="Link" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{8EB0951B-536C-46AF-A6D3-CAE4AA26E548}" name="Added to map?" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{EEB18F33-2716-411A-B364-7A12EF0925D3}" name="Link" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{D5EF4736-10A8-4D6A-B209-5897B4049F98}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1163,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DB3DEB-0EB8-4FD3-9EF9-F81EADE7405E}">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,10 +1195,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1206,10 +1212,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1223,7 +1229,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1237,7 +1243,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1251,10 +1257,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1268,10 +1274,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1285,10 +1291,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1302,86 +1308,86 @@
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9" t="s">
         <v>207</v>
       </c>
-      <c r="B9" t="s">
-        <v>210</v>
-      </c>
       <c r="C9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1" t="b">
         <v>0</v>
@@ -1389,126 +1395,126 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C14" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E15" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E16" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E17" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C18" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E18" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B20" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C20" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E20" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C21" s="1" t="b">
         <v>0</v>
@@ -1516,66 +1522,66 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C25" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C26" s="1" t="b">
         <v>0</v>
@@ -1583,7 +1589,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -1592,117 +1598,117 @@
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E27" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B28" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C28" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E28" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C29" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E29" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C30" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E30" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C31" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E31" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C32" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E32" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C33" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C34" s="1" t="b">
         <v>0</v>
@@ -1710,27 +1716,27 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B35" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C35" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E35" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C36" s="1" t="b">
         <v>0</v>
@@ -1738,44 +1744,44 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B37" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C37" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E37" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C38" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E38" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C39" s="1" t="b">
         <v>0</v>
@@ -1783,10 +1789,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C40" s="1" t="b">
         <v>0</v>
@@ -1794,27 +1800,27 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E41" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C42" s="1" t="b">
         <v>1</v>
@@ -1822,50 +1828,50 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C43" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B44" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C44" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E44" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B45" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C45" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E45" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1873,156 +1879,156 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C46" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E46" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C47" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E47" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C49" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E49" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C50" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B51" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C51" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E51" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C52" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C53" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B54" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C54" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C55" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B56" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C56" s="1" t="b">
         <v>0</v>
@@ -2030,27 +2036,27 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B57" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C57" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E57" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C58" s="1" t="b">
         <v>0</v>
@@ -2058,19 +2064,19 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C59" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E59" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2078,24 +2084,24 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C60" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E60" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C61" s="1" t="b">
         <v>0</v>
@@ -2103,10 +2109,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B62" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C62" s="1" t="b">
         <v>0</v>
@@ -2114,61 +2120,61 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B63" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C63" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E63" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B64" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C64" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E64" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B65" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C65" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E65" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C66" s="1" t="b">
         <v>0</v>
@@ -2176,58 +2182,58 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B67" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C67" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C68" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E68" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B69" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C69" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E69" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B70" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C70" s="1" t="b">
         <v>0</v>
@@ -2235,24 +2241,24 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B71" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C71" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B72" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C72" s="1" t="b">
         <v>0</v>
@@ -2260,61 +2266,61 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B73" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C73" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E73" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B74" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C74" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E74" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B75" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C75" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E75" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B76" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C76" s="1" t="b">
         <v>1</v>
@@ -2322,41 +2328,41 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B77" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C77" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>168</v>
+        <v>191</v>
       </c>
       <c r="E77" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B78" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C78" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="E78" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B79" t="s">
         <v>32</v>
@@ -2365,145 +2371,139 @@
         <v>1</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E79" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B80" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C80" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E80" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="B81" t="s">
-        <v>30</v>
+        <v>131</v>
       </c>
       <c r="C81" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E81" t="s">
-        <v>185</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="B82" t="s">
-        <v>133</v>
+        <v>22</v>
       </c>
       <c r="C82" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="E82" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="B83" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="C83" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E83" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>128</v>
+        <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>129</v>
+        <v>21</v>
       </c>
       <c r="C84" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>177</v>
+      <c r="D84" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E84" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>20</v>
+        <v>210</v>
       </c>
       <c r="B85" t="s">
-        <v>21</v>
+        <v>211</v>
       </c>
       <c r="C85" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>165</v>
+        <v>0</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="E85" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>213</v>
+        <v>27</v>
       </c>
       <c r="B86" t="s">
-        <v>214</v>
+        <v>28</v>
       </c>
       <c r="C86" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="E86" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B87" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C87" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="E87" t="s">
-        <v>185</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B88" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C88" s="1" t="b">
         <v>0</v>
@@ -2511,30 +2511,53 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>18</v>
+        <v>205</v>
       </c>
       <c r="B89" t="s">
-        <v>19</v>
+        <v>203</v>
       </c>
       <c r="C89" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E89" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="B90" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="C90" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="E90" t="s">
-        <v>185</v>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>235</v>
+      </c>
+      <c r="B91" t="s">
+        <v>233</v>
+      </c>
+      <c r="C91" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E91" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2548,13 +2571,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"WIP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="iconSet" priority="5">
@@ -2573,7 +2596,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D85" r:id="rId1" xr:uid="{27C35F13-2332-4ADD-AE84-E0315758E4E1}"/>
+    <hyperlink ref="D84" r:id="rId1" xr:uid="{27C35F13-2332-4ADD-AE84-E0315758E4E1}"/>
     <hyperlink ref="D60" r:id="rId2" xr:uid="{4DCA43D3-DFC4-4C5D-A2F4-D33BA5444378}"/>
     <hyperlink ref="D46" r:id="rId3" xr:uid="{1177B9A5-E58D-41B0-B8B0-8BC9E84B3ECD}"/>
     <hyperlink ref="D37" r:id="rId4" xr:uid="{F42D7F6F-9FE8-4E54-8FBE-DDEEAD186D0C}"/>

</xml_diff>